<commit_message>
latest data after running sbi portfolio change engine
</commit_message>
<xml_diff>
--- a/mf-intelligence/data/separated_files/sbi/SBI Banking And Financial Services Fund/SBI Banking And Financial Services Fund_Apr_2025.xlsx
+++ b/mf-intelligence/data/separated_files/sbi/SBI Banking And Financial Services Fund/SBI Banking And Financial Services Fund_Apr_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,867 +436,633 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Name of the Instrument / Issuer</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 1</t>
+          <t>ISIN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Name of the Instrument / Issuer</t>
+          <t>Rating / Industry^</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ISIN</t>
+          <t>Quantity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Rating / Industry^</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Market value
 (Rs. in Lakhs)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>% to AUM</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>YTM %</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>YTC % ##</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Notes &amp; Symbols</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HDFC Bank Ltd.</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100006</t>
+          <t>INE040A01034</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HDFC Bank Ltd.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>INE040A01034</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>11014715</v>
+      </c>
+      <c r="E2" t="n">
+        <v>212033.26</v>
+      </c>
       <c r="F2" t="n">
-        <v>11014715</v>
-      </c>
-      <c r="G2" t="n">
-        <v>212033.26</v>
-      </c>
-      <c r="H2" t="n">
         <v>27.72</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ICICI Bank Ltd.</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100012</t>
+          <t>INE090A01021</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ICICI Bank Ltd.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>INE090A01021</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>6035814</v>
+      </c>
+      <c r="E3" t="n">
+        <v>86131.07000000001</v>
+      </c>
       <c r="F3" t="n">
-        <v>6035814</v>
-      </c>
-      <c r="G3" t="n">
-        <v>86131.07000000001</v>
-      </c>
-      <c r="H3" t="n">
         <v>11.26</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Axis Bank Ltd.</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>100024</t>
+          <t>INE238A01034</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Axis Bank Ltd.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>INE238A01034</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D4" t="n">
+        <v>6285625</v>
+      </c>
+      <c r="E4" t="n">
+        <v>74484.66</v>
+      </c>
       <c r="F4" t="n">
-        <v>6285625</v>
-      </c>
-      <c r="G4" t="n">
-        <v>74484.66</v>
-      </c>
-      <c r="H4" t="n">
         <v>9.74</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kotak Mahindra Bank Ltd.</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>100104</t>
+          <t>INE237A01028</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Kotak Mahindra Bank Ltd.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>INE237A01028</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D5" t="n">
+        <v>3191554</v>
+      </c>
+      <c r="E5" t="n">
+        <v>70472.7</v>
+      </c>
       <c r="F5" t="n">
-        <v>3191554</v>
-      </c>
-      <c r="G5" t="n">
-        <v>70472.7</v>
-      </c>
-      <c r="H5" t="n">
         <v>9.210000000000001</v>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>100010</t>
+          <t>INE062A01020</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>INE062A01020</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D6" t="n">
+        <v>6005364</v>
+      </c>
+      <c r="E6" t="n">
+        <v>47361.3</v>
+      </c>
       <c r="F6" t="n">
-        <v>6005364</v>
-      </c>
-      <c r="G6" t="n">
-        <v>47361.3</v>
-      </c>
-      <c r="H6" t="n">
         <v>6.19</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HDFC Life Insurance Company Ltd.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>100706</t>
+          <t>INE795G01014</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HDFC Life Insurance Company Ltd.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>INE795G01014</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
           <t>Insurance</t>
         </is>
       </c>
+      <c r="D7" t="n">
+        <v>4274765</v>
+      </c>
+      <c r="E7" t="n">
+        <v>31791.43</v>
+      </c>
       <c r="F7" t="n">
-        <v>4274765</v>
-      </c>
-      <c r="G7" t="n">
-        <v>31791.43</v>
-      </c>
-      <c r="H7" t="n">
         <v>4.16</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Max Financial Services Ltd.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>100107</t>
+          <t>INE180A01020</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Max Financial Services Ltd.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>INE180A01020</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
           <t>Insurance</t>
         </is>
       </c>
+      <c r="D8" t="n">
+        <v>2018698</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26344.01</v>
+      </c>
       <c r="F8" t="n">
-        <v>2018698</v>
-      </c>
-      <c r="G8" t="n">
-        <v>26344.01</v>
-      </c>
-      <c r="H8" t="n">
         <v>3.44</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Muthoot Finance Ltd.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>100231</t>
+          <t>INE414G01012</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Muthoot Finance Ltd.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>INE414G01012</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D9" t="n">
+        <v>1129041</v>
+      </c>
+      <c r="E9" t="n">
+        <v>24499.06</v>
+      </c>
       <c r="F9" t="n">
-        <v>1129041</v>
-      </c>
-      <c r="G9" t="n">
-        <v>24499.06</v>
-      </c>
-      <c r="H9" t="n">
         <v>3.2</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bank of Baroda</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>100092</t>
+          <t>INE028A01039</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>INE028A01039</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D10" t="n">
+        <v>8985585</v>
+      </c>
+      <c r="E10" t="n">
+        <v>22457.67</v>
+      </c>
       <c r="F10" t="n">
-        <v>8985585</v>
-      </c>
-      <c r="G10" t="n">
-        <v>22457.67</v>
-      </c>
-      <c r="H10" t="n">
         <v>2.94</v>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SBI Cards &amp; Payment Services Ltd.</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>101119</t>
+          <t>INE018E01016</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SBI Cards &amp; Payment Services Ltd.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>INE018E01016</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D11" t="n">
+        <v>2033600</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17764.51</v>
+      </c>
       <c r="F11" t="n">
-        <v>2033600</v>
-      </c>
-      <c r="G11" t="n">
-        <v>17764.51</v>
-      </c>
-      <c r="H11" t="n">
         <v>2.32</v>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Aptus Value Housing Finance India Ltd.</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>101488</t>
+          <t>INE852O01025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Aptus Value Housing Finance India Ltd.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>INE852O01025</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D12" t="n">
+        <v>5481117</v>
+      </c>
+      <c r="E12" t="n">
+        <v>17465.58</v>
+      </c>
       <c r="F12" t="n">
-        <v>5481117</v>
-      </c>
-      <c r="G12" t="n">
-        <v>17465.58</v>
-      </c>
-      <c r="H12" t="n">
         <v>2.28</v>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Nippon Life India Asset Management Ltd.</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>100701</t>
+          <t>INE298J01013</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Nippon Life India Asset Management Ltd.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>INE298J01013</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
           <t>Capital Markets</t>
         </is>
       </c>
+      <c r="D13" t="n">
+        <v>2667235</v>
+      </c>
+      <c r="E13" t="n">
+        <v>17035.63</v>
+      </c>
       <c r="F13" t="n">
-        <v>2667235</v>
-      </c>
-      <c r="G13" t="n">
-        <v>17035.63</v>
-      </c>
-      <c r="H13" t="n">
         <v>2.23</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Power Finance Corporation Ltd.</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>100194</t>
+          <t>INE134E01011</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Power Finance Corporation Ltd.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>INE134E01011</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D14" t="n">
+        <v>4155779</v>
+      </c>
+      <c r="E14" t="n">
+        <v>16930.64</v>
+      </c>
       <c r="F14" t="n">
-        <v>4155779</v>
-      </c>
-      <c r="G14" t="n">
-        <v>16930.64</v>
-      </c>
-      <c r="H14" t="n">
         <v>2.21</v>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Bank of India</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>100361</t>
+          <t>INE084A01016</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bank of India</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>INE084A01016</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D15" t="n">
+        <v>14190730</v>
+      </c>
+      <c r="E15" t="n">
+        <v>16340.63</v>
+      </c>
       <c r="F15" t="n">
-        <v>14190730</v>
-      </c>
-      <c r="G15" t="n">
-        <v>16340.63</v>
-      </c>
-      <c r="H15" t="n">
         <v>2.14</v>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>City Union Bank Ltd.</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>100256</t>
+          <t>INE491A01021</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>City Union Bank Ltd.</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>INE491A01021</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
           <t>Banks</t>
         </is>
       </c>
+      <c r="D16" t="n">
+        <v>5281475</v>
+      </c>
+      <c r="E16" t="n">
+        <v>9324.969999999999</v>
+      </c>
       <c r="F16" t="n">
-        <v>5281475</v>
-      </c>
-      <c r="G16" t="n">
-        <v>9324.969999999999</v>
-      </c>
-      <c r="H16" t="n">
         <v>1.22</v>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Aditya Birla Capital Ltd.</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>100665</t>
+          <t>INE674K01013</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Aditya Birla Capital Ltd.</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INE674K01013</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D17" t="n">
+        <v>4519577</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8874.639999999999</v>
+      </c>
       <c r="F17" t="n">
-        <v>4519577</v>
-      </c>
-      <c r="G17" t="n">
-        <v>8874.639999999999</v>
-      </c>
-      <c r="H17" t="n">
         <v>1.16</v>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Cholamandalam Financial Holdings Ltd.</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>100220</t>
+          <t>INE149A01033</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Cholamandalam Financial Holdings Ltd.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>INE149A01033</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D18" t="n">
+        <v>405052</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7550.57</v>
+      </c>
       <c r="F18" t="n">
-        <v>405052</v>
-      </c>
-      <c r="G18" t="n">
-        <v>7550.57</v>
-      </c>
-      <c r="H18" t="n">
         <v>0.99</v>
       </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Manappuram Finance Ltd.</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>100046</t>
+          <t>INE522D01027</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Manappuram Finance Ltd.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>INE522D01027</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D19" t="n">
+        <v>2994974</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6913.9</v>
+      </c>
       <c r="F19" t="n">
-        <v>2994974</v>
-      </c>
-      <c r="G19" t="n">
-        <v>6913.9</v>
-      </c>
-      <c r="H19" t="n">
         <v>0.9</v>
       </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CARE Ratings Ltd.</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>100073</t>
+          <t>INE752H01013</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CARE Ratings Ltd.</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>INE752H01013</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
           <t>Capital Markets</t>
         </is>
       </c>
+      <c r="D20" t="n">
+        <v>538620</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6512.99</v>
+      </c>
       <c r="F20" t="n">
-        <v>538620</v>
-      </c>
-      <c r="G20" t="n">
-        <v>6512.99</v>
-      </c>
-      <c r="H20" t="n">
         <v>0.85</v>
       </c>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ICRA Ltd.</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>100160</t>
+          <t>INE725G01011</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ICRA Ltd.</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>INE725G01011</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
           <t>Capital Markets</t>
         </is>
       </c>
+      <c r="D21" t="n">
+        <v>113760</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6323.92</v>
+      </c>
       <c r="F21" t="n">
-        <v>113760</v>
-      </c>
-      <c r="G21" t="n">
-        <v>6323.92</v>
-      </c>
-      <c r="H21" t="n">
         <v>0.83</v>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CRISIL Ltd.</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>100235</t>
+          <t>INE007A01025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CRISIL Ltd.</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>INE007A01025</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D22" t="n">
+        <v>122912</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5472.9</v>
+      </c>
       <c r="F22" t="n">
-        <v>122912</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5472.9</v>
-      </c>
-      <c r="H22" t="n">
         <v>0.72</v>
       </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SBFC Finance Ltd.</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>101929</t>
+          <t>INE423Y01016</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SBFC Finance Ltd.</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>INE423Y01016</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
           <t>Finance</t>
         </is>
       </c>
+      <c r="D23" t="n">
+        <v>3033160</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3101.41</v>
+      </c>
       <c r="F23" t="n">
-        <v>3033160</v>
-      </c>
-      <c r="G23" t="n">
-        <v>3101.41</v>
-      </c>
-      <c r="H23" t="n">
         <v>0.41</v>
       </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>182 DAY T-BILL 05.06.25</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1801270</t>
+          <t>IN002024Y340</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>182 DAY T-BILL 05.06.25</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>IN002024Y340</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
           <t>Sovereign</t>
         </is>
       </c>
+      <c r="D24" t="n">
+        <v>500000</v>
+      </c>
+      <c r="E24" t="n">
+        <v>497.2</v>
+      </c>
       <c r="F24" t="n">
-        <v>500000</v>
-      </c>
-      <c r="G24" t="n">
-        <v>497.2</v>
-      </c>
-      <c r="H24" t="n">
         <v>0.06</v>
       </c>
-      <c r="I24" t="n">
-        <v>5.8703</v>
-      </c>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>